<commit_message>
Remove year column from obs data where not needed.
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/ObsPloschuk2021.xlsx
+++ b/Tests/Validation/Canola/ObsPloschuk2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilhuber\NextGen\ApsimX\Tests\Validation\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E07C6B-6283-458A-81E3-1E3FC23EF8E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B7C8FA-AE9A-43F2-95BC-323A83DDBB69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="2430" windowWidth="28800" windowHeight="13050" activeTab="3" xr2:uid="{03D29272-A8D3-49D2-9408-6969D9C41BBD}"/>
+    <workbookView xWindow="10080" yWindow="2430" windowWidth="28800" windowHeight="13050" activeTab="4" xr2:uid="{03D29272-A8D3-49D2-9408-6969D9C41BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Canola" sheetId="3" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="TimeSeries" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">LAI_at_end_treatment!$A$1:$G$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RUE_at_end_treatment!$A$1:$F$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TimeSeries!$A$1:$H$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">LAI_at_end_treatment!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RUE_at_end_treatment!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TimeSeries!$A$1:$G$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="38">
   <si>
     <t>LAI</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Late_WL</t>
-  </si>
-  <si>
-    <t>Biomass_kgha</t>
   </si>
   <si>
     <t>Canola.Leaf.LAI</t>
@@ -924,10 +921,10 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -936,10 +933,10 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
@@ -1273,20 +1270,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71534395-E1B7-48CE-9FD5-CA31AE8A997A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1294,70 +1291,61 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="str">
-        <f>"Exp_1_"&amp;E2</f>
+        <f>"Exp_1_"&amp;D2</f>
         <v>Exp_1_Control</v>
       </c>
       <c r="B2" s="1">
         <v>42999</v>
       </c>
-      <c r="C2">
-        <v>2017</v>
+      <c r="C2" t="s">
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>2.9640287769784099</v>
       </c>
       <c r="F2">
-        <v>2.9640287769784099</v>
-      </c>
-      <c r="G2">
         <v>0.54827507577720203</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A11" si="0">"Exp_1_"&amp;E3</f>
+        <f t="shared" ref="A3:A11" si="0">"Exp_1_"&amp;D3</f>
         <v>Exp_1_Early_WL</v>
       </c>
       <c r="B3" s="1">
         <v>42999</v>
       </c>
-      <c r="C3">
-        <v>2017</v>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
         <v>26</v>
       </c>
+      <c r="E3">
+        <v>1.0647482014388401</v>
+      </c>
       <c r="F3">
-        <v>1.0647482014388401</v>
-      </c>
-      <c r="G3">
         <v>0.59811826448422634</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1365,23 +1353,20 @@
       <c r="B4" s="1">
         <v>43029</v>
       </c>
-      <c r="C4">
-        <v>2017</v>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>3.0791366906474802</v>
       </c>
       <c r="F4">
-        <v>3.0791366906474802</v>
-      </c>
-      <c r="G4">
         <v>1.0467069628473786</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1389,23 +1374,20 @@
       <c r="B5" s="1">
         <v>43029</v>
       </c>
-      <c r="C5">
-        <v>2017</v>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
         <v>26</v>
       </c>
+      <c r="E5">
+        <v>1.72661870503597</v>
+      </c>
       <c r="F5">
-        <v>1.72661870503597</v>
-      </c>
-      <c r="G5">
         <v>0.49843188707017699</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1413,23 +1395,20 @@
       <c r="B6" s="1">
         <v>43029</v>
       </c>
-      <c r="C6">
-        <v>2017</v>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
         <v>27</v>
       </c>
+      <c r="E6">
+        <v>0.115107913669064</v>
+      </c>
       <c r="F6">
-        <v>0.115107913669064</v>
-      </c>
-      <c r="G6">
         <v>9.9686377414031968E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1437,23 +1416,20 @@
       <c r="B7" s="1">
         <v>43375</v>
       </c>
-      <c r="C7">
-        <v>2018</v>
+      <c r="C7" t="s">
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>3.94244604316546</v>
       </c>
       <c r="F7">
-        <v>3.94244604316546</v>
-      </c>
-      <c r="G7">
         <v>1.495295661210549</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1461,23 +1437,20 @@
       <c r="B8" s="1">
         <v>43375</v>
       </c>
-      <c r="C8">
-        <v>2018</v>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
         <v>26</v>
       </c>
+      <c r="E8">
+        <v>0.23021582733812801</v>
+      </c>
       <c r="F8">
-        <v>0.23021582733812801</v>
-      </c>
-      <c r="G8">
         <v>0.14952956612105486</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1485,23 +1458,20 @@
       <c r="B9" s="1">
         <v>43397</v>
       </c>
-      <c r="C9">
-        <v>2018</v>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>3.28057553956834</v>
       </c>
       <c r="F9">
-        <v>3.28057553956834</v>
-      </c>
-      <c r="G9">
         <v>9.9686377414031635E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1509,23 +1479,20 @@
       <c r="B10" s="1">
         <v>43397</v>
       </c>
-      <c r="C10">
-        <v>2018</v>
+      <c r="C10" t="s">
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
         <v>26</v>
       </c>
+      <c r="E10">
+        <v>0.74820143884891899</v>
+      </c>
       <c r="F10">
-        <v>0.74820143884891899</v>
-      </c>
-      <c r="G10">
         <v>0.44858869836315446</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1533,19 +1500,16 @@
       <c r="B11" s="1">
         <v>43397</v>
       </c>
-      <c r="C11">
-        <v>2018</v>
+      <c r="C11" t="s">
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
         <v>27</v>
       </c>
+      <c r="E11">
+        <v>0.37410071942445799</v>
+      </c>
       <c r="F11">
-        <v>0.37410071942445799</v>
-      </c>
-      <c r="G11">
         <v>0.14952956612105495</v>
       </c>
     </row>
@@ -1556,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9952680-0C64-4320-B545-A57AD469F530}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1568,7 +1532,7 @@
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1576,61 +1540,52 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="str">
-        <f>"Exp_1_"&amp;D2</f>
+        <f>"Exp_1_"&amp;C2</f>
         <v>Exp_1_Control</v>
       </c>
       <c r="B2" s="1">
         <v>42999</v>
       </c>
-      <c r="C2">
-        <v>2017</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>0.78160919540229901</v>
       </c>
       <c r="E2">
-        <v>0.78160919540229901</v>
-      </c>
-      <c r="F2">
         <v>0.11945177983233236</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A21" si="0">"Exp_1_"&amp;D3</f>
+        <f t="shared" ref="A3:A21" si="0">"Exp_1_"&amp;C3</f>
         <v>Exp_1_Early_WL</v>
       </c>
       <c r="B3" s="1">
         <v>42999</v>
       </c>
-      <c r="C3">
-        <v>2017</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
+      <c r="D3">
+        <v>0.34482758620689502</v>
+      </c>
       <c r="E3">
-        <v>0.34482758620689502</v>
-      </c>
-      <c r="F3">
         <v>0.11945177983233755</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1638,20 +1593,17 @@
       <c r="B4" s="1">
         <v>43015</v>
       </c>
-      <c r="C4">
-        <v>2017</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>2.1609195402298802</v>
       </c>
       <c r="E4">
-        <v>2.1609195402298802</v>
-      </c>
-      <c r="F4">
         <v>0.19908629972055614</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1659,20 +1611,17 @@
       <c r="B5" s="1">
         <v>43015</v>
       </c>
-      <c r="C5">
-        <v>2017</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
+      <c r="D5">
+        <v>1.3103448275862</v>
+      </c>
       <c r="E5">
-        <v>1.3103448275862</v>
-      </c>
-      <c r="F5">
         <v>0.75652793893812631</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1680,20 +1629,17 @@
       <c r="B6" s="1">
         <v>43042</v>
       </c>
-      <c r="C6">
-        <v>2017</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
         <v>0.27872081960877643</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1701,20 +1647,17 @@
       <c r="B7" s="1">
         <v>43042</v>
       </c>
-      <c r="C7">
-        <v>2017</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
+      <c r="D7">
+        <v>2.2298850574712601</v>
+      </c>
       <c r="E7">
-        <v>2.2298850574712601</v>
-      </c>
-      <c r="F7">
         <v>1.0750660184910201</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1722,20 +1665,17 @@
       <c r="B8" s="1">
         <v>43015</v>
       </c>
-      <c r="C8">
-        <v>2017</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>1.9540229885057401</v>
       </c>
       <c r="E8">
-        <v>1.9540229885057401</v>
-      </c>
-      <c r="F8">
         <v>0.23890355966467472</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1743,20 +1683,17 @@
       <c r="B9" s="1">
         <v>43015</v>
       </c>
-      <c r="C9">
-        <v>2017</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
+      <c r="D9">
+        <v>1.56321839080459</v>
+      </c>
       <c r="E9">
-        <v>1.56321839080459</v>
-      </c>
-      <c r="F9">
         <v>7.9634519888236444E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1764,20 +1701,17 @@
       <c r="B10" s="1">
         <v>43040</v>
       </c>
-      <c r="C10">
-        <v>2017</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
         <v>0.27872081960877643</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1785,20 +1719,17 @@
       <c r="B11" s="1">
         <v>43040</v>
       </c>
-      <c r="C11">
-        <v>2017</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>27</v>
       </c>
+      <c r="D11">
+        <v>1.9310344827586201</v>
+      </c>
       <c r="E11">
-        <v>1.9310344827586201</v>
-      </c>
-      <c r="F11">
         <v>0.47780711932933256</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1806,20 +1737,17 @@
       <c r="B12" s="1">
         <v>43361</v>
       </c>
-      <c r="C12">
-        <v>2018</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>2.7126436781609198</v>
       </c>
       <c r="E12">
-        <v>2.7126436781609198</v>
-      </c>
-      <c r="F12">
         <v>0.6370761591057893</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1827,20 +1755,17 @@
       <c r="B13" s="1">
         <v>43361</v>
       </c>
-      <c r="C13">
-        <v>2018</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
+      <c r="D13">
+        <v>1.1954022988505699</v>
+      </c>
       <c r="E13">
-        <v>1.1954022988505699</v>
-      </c>
-      <c r="F13">
         <v>0.23890355966467511</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1848,20 +1773,17 @@
       <c r="B14" s="1">
         <v>43386.5</v>
       </c>
-      <c r="C14">
-        <v>2018</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>1.28735632183908</v>
       </c>
       <c r="E14">
-        <v>1.28735632183908</v>
-      </c>
-      <c r="F14">
         <v>0.39817259944111377</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:5">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1869,20 +1791,17 @@
       <c r="B15" s="1">
         <v>43386.5</v>
       </c>
-      <c r="C15">
-        <v>2018</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
+      <c r="D15">
+        <v>0.390804597701148</v>
+      </c>
       <c r="E15">
-        <v>0.390804597701148</v>
-      </c>
-      <c r="F15">
         <v>7.9634519888224425E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1890,20 +1809,17 @@
       <c r="B16" s="1">
         <v>43407</v>
       </c>
-      <c r="C16">
-        <v>2018</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>2.13793103448275</v>
       </c>
       <c r="E16">
-        <v>2.13793103448275</v>
-      </c>
-      <c r="F16">
         <v>0.71671067899402496</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1911,20 +1827,17 @@
       <c r="B17" s="1">
         <v>43407</v>
       </c>
-      <c r="C17">
-        <v>2018</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>26</v>
       </c>
+      <c r="D17">
+        <v>2.6666666666666599</v>
+      </c>
       <c r="E17">
-        <v>2.6666666666666599</v>
-      </c>
-      <c r="F17">
         <v>0.39817259944113148</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1932,20 +1845,17 @@
       <c r="B18" s="1">
         <v>43383</v>
       </c>
-      <c r="C18">
-        <v>2018</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <v>1.86206896551724</v>
       </c>
       <c r="E18">
-        <v>1.86206896551724</v>
-      </c>
-      <c r="F18">
         <v>0.35835533949701248</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1953,20 +1863,17 @@
       <c r="B19" s="1">
         <v>43383</v>
       </c>
-      <c r="C19">
-        <v>2018</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
+      <c r="D19">
+        <v>1.12643678160919</v>
+      </c>
       <c r="E19">
-        <v>1.12643678160919</v>
-      </c>
-      <c r="F19">
         <v>0.15926903977645598</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1974,20 +1881,17 @@
       <c r="B20" s="1">
         <v>43406.5</v>
       </c>
-      <c r="C20">
-        <v>2018</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>2.13793103448275</v>
       </c>
       <c r="E20">
-        <v>2.13793103448275</v>
-      </c>
-      <c r="F20">
         <v>0.71671067899402496</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1995,16 +1899,13 @@
       <c r="B21" s="1">
         <v>43406.5</v>
       </c>
-      <c r="C21">
-        <v>2018</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
+      <c r="D21">
+        <v>0.78160919540229901</v>
+      </c>
       <c r="E21">
-        <v>0.78160919540229901</v>
-      </c>
-      <c r="F21">
         <v>0.2787208196087812</v>
       </c>
     </row>
@@ -2016,19 +1917,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCDE50D-DC28-4398-95CA-92F7BC129FD5}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2036,102 +1937,87 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
       <c r="G1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="str">
+        <f>"Exp_1_"&amp;C2</f>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>42985</v>
+      </c>
+      <c r="F2">
+        <v>0.57788944723618096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A66" si="0">"Exp_1_"&amp;C3</f>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <f>$E$2+D3</f>
+        <v>42994</v>
+      </c>
+      <c r="F3">
+        <v>0.91959798994974795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="str">
-        <f>"Exp_1_"&amp;D2</f>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <v>2017</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>42985</v>
-      </c>
-      <c r="G2">
-        <v>0.57788944723618096</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A66" si="0">"Exp_1_"&amp;D3</f>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>2017</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <f>$F$2+E3</f>
-        <v>42994</v>
-      </c>
-      <c r="G3">
-        <v>0.91959798994974795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
-        <v>2017</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>33</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F9" si="1">$F$2+E4</f>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E9" si="1">$E$2+D4</f>
         <v>43018</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>0.95477386934673303</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2139,24 +2025,21 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5">
-        <v>2017</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
         <v>46</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E5" s="1">
         <f t="shared" si="1"/>
         <v>43031</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>0.96482412060301503</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:7">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2164,24 +2047,21 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
-        <v>2017</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3">
         <v>49</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E6" s="1">
         <f t="shared" si="1"/>
         <v>43034</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>0.904522613065326</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:7">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2189,24 +2069,21 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>2017</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3">
         <v>57</v>
       </c>
-      <c r="F7" s="1">
+      <c r="E7" s="1">
         <f t="shared" si="1"/>
         <v>43042</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <v>0.89447236180904399</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:7">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2214,24 +2091,21 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8">
-        <v>2017</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3">
         <v>66</v>
       </c>
-      <c r="F8" s="1">
+      <c r="E8" s="1">
         <f t="shared" si="1"/>
         <v>43051</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>0.82412060301507495</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:7">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2239,24 +2113,21 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
-        <v>2017</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
         <v>71</v>
       </c>
-      <c r="F9" s="1">
+      <c r="E9" s="1">
         <f t="shared" si="1"/>
         <v>43056</v>
       </c>
-      <c r="G9">
+      <c r="F9">
         <v>0.67839195979899403</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:7">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2264,24 +2135,21 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>2017</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3">
+      <c r="D10" s="3">
         <v>10</v>
       </c>
-      <c r="F10" s="1">
-        <f>$F$2+E10</f>
+      <c r="E10" s="1">
+        <f>$E$2+D10</f>
         <v>42995</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <v>0.56281407035175901</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:7">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2289,24 +2157,21 @@
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11">
-        <v>2017</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="3">
+      <c r="D11" s="3">
         <v>16</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F17" si="2">$F$2+E11</f>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11:E17" si="2">$E$2+D11</f>
         <v>43001</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <v>0.41708542713567798</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:7">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2314,24 +2179,21 @@
       <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12">
-        <v>2017</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="3">
+      <c r="D12" s="3">
         <v>33</v>
       </c>
-      <c r="F12" s="1">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>43018</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>0.86934673366834103</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:7">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2339,24 +2201,21 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
-        <v>2017</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="3">
+      <c r="D13" s="3">
         <v>46</v>
       </c>
-      <c r="F13" s="1">
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>43031</v>
       </c>
-      <c r="G13">
+      <c r="F13">
         <v>0.80904522613065299</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:7">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2364,24 +2223,21 @@
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C14">
-        <v>2017</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="3">
+      <c r="D14" s="3">
         <v>50</v>
       </c>
-      <c r="F14" s="1">
+      <c r="E14" s="1">
         <f t="shared" si="2"/>
         <v>43035</v>
       </c>
-      <c r="G14">
+      <c r="F14">
         <v>0.85929648241206003</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:7">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2389,24 +2245,21 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15">
-        <v>2017</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="3">
+      <c r="D15" s="3">
         <v>57</v>
       </c>
-      <c r="F15" s="1">
+      <c r="E15" s="1">
         <f t="shared" si="2"/>
         <v>43042</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <v>0.81407035175879405</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:7">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2414,24 +2267,21 @@
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16">
-        <v>2017</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="3">
+      <c r="D16" s="3">
         <v>66</v>
       </c>
-      <c r="F16" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>43051</v>
       </c>
-      <c r="G16">
+      <c r="F16">
         <v>0.85929648241206003</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:6">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2439,24 +2289,21 @@
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
-        <v>2017</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="3">
+      <c r="D17" s="3">
         <v>72</v>
       </c>
-      <c r="F17" s="1">
+      <c r="E17" s="1">
         <f t="shared" si="2"/>
         <v>43057</v>
       </c>
-      <c r="G17">
+      <c r="F17">
         <v>0.80904522613065299</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:6">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2464,24 +2311,21 @@
       <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18">
-        <v>2017</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3">
+      <c r="D18" s="3">
         <v>32</v>
       </c>
-      <c r="F18" s="1">
-        <f>$F$2+E18</f>
+      <c r="E18" s="1">
+        <f>$E$2+D18</f>
         <v>43017</v>
       </c>
-      <c r="G18">
+      <c r="F18">
         <v>0.904522613065326</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:6">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2489,24 +2333,21 @@
       <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="C19">
-        <v>2017</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3">
+      <c r="D19" s="3">
         <v>46</v>
       </c>
-      <c r="F19" s="1">
-        <f t="shared" ref="F19:F23" si="3">$F$2+E19</f>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E23" si="3">$E$2+D19</f>
         <v>43031</v>
       </c>
-      <c r="G19">
+      <c r="F19">
         <v>0.51758793969849204</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:6">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2514,24 +2355,21 @@
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20">
-        <v>2017</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="3">
+      <c r="D20" s="3">
         <v>50</v>
       </c>
-      <c r="F20" s="1">
+      <c r="E20" s="1">
         <f t="shared" si="3"/>
         <v>43035</v>
       </c>
-      <c r="G20">
+      <c r="F20">
         <v>0.32663316582914498</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:6">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2539,24 +2377,21 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
-        <v>2017</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="3">
+      <c r="D21" s="3">
         <v>57</v>
       </c>
-      <c r="F21" s="1">
+      <c r="E21" s="1">
         <f t="shared" si="3"/>
         <v>43042</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>0.33668341708542598</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:6">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2564,24 +2399,21 @@
       <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="C22">
-        <v>2017</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="3">
+      <c r="D22" s="3">
         <v>67</v>
       </c>
-      <c r="F22" s="1">
+      <c r="E22" s="1">
         <f t="shared" si="3"/>
         <v>43052</v>
       </c>
-      <c r="G22">
+      <c r="F22">
         <v>0.46733668341708501</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:6">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2589,24 +2421,21 @@
       <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C23">
-        <v>2017</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="3">
+      <c r="D23" s="3">
         <v>72</v>
       </c>
-      <c r="F23" s="1">
+      <c r="E23" s="1">
         <f t="shared" si="3"/>
         <v>43057</v>
       </c>
-      <c r="G23">
+      <c r="F23">
         <v>0.34170854271356699</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:6">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2614,24 +2443,20 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C24">
-        <v>2018</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="4">
+      <c r="E24" s="4">
         <v>43361</v>
       </c>
-      <c r="G24">
+      <c r="F24">
         <v>0.25974025974025999</v>
       </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2639,24 +2464,21 @@
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>2018</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
-        <f>$F$24+E25</f>
+      <c r="E25" s="1">
+        <f>$E$24+D25</f>
         <v>43369</v>
       </c>
-      <c r="G25">
+      <c r="F25">
         <v>0.74025974025973995</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:6">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2664,24 +2486,21 @@
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
-        <v>2018</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
         <v>16</v>
       </c>
-      <c r="F26" s="1">
-        <f t="shared" ref="F26:F33" si="4">$F$24+E26</f>
+      <c r="E26" s="1">
+        <f t="shared" ref="E26:E33" si="4">$E$24+D26</f>
         <v>43377</v>
       </c>
-      <c r="G26">
+      <c r="F26">
         <v>0.92207792207792205</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:6">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2689,24 +2508,21 @@
       <c r="B27" t="s">
         <v>24</v>
       </c>
-      <c r="C27">
-        <v>2018</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3">
         <v>19</v>
       </c>
-      <c r="F27" s="1">
+      <c r="E27" s="1">
         <f t="shared" si="4"/>
         <v>43380</v>
       </c>
-      <c r="G27">
+      <c r="F27">
         <v>0.89610389610389596</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:6">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2714,24 +2530,21 @@
       <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C28">
-        <v>2018</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="3">
-        <v>24</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="3">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1">
         <f t="shared" si="4"/>
         <v>43385</v>
       </c>
-      <c r="G28">
+      <c r="F28">
         <v>0.92857142857142905</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:6">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2739,24 +2552,21 @@
       <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="C29">
-        <v>2018</v>
-      </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="3">
         <v>30</v>
       </c>
-      <c r="F29" s="1">
+      <c r="E29" s="1">
         <f t="shared" si="4"/>
         <v>43391</v>
       </c>
-      <c r="G29">
+      <c r="F29">
         <v>0.95454545454545503</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:6">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2764,24 +2574,21 @@
       <c r="B30" t="s">
         <v>24</v>
       </c>
-      <c r="C30">
-        <v>2018</v>
-      </c>
-      <c r="D30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="3">
         <v>43</v>
       </c>
-      <c r="F30" s="1">
+      <c r="E30" s="1">
         <f t="shared" si="4"/>
         <v>43404</v>
       </c>
-      <c r="G30">
+      <c r="F30">
         <v>0.84415584415584399</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:6">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2789,24 +2596,21 @@
       <c r="B31" t="s">
         <v>24</v>
       </c>
-      <c r="C31">
-        <v>2018</v>
-      </c>
-      <c r="D31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="3">
         <v>52</v>
       </c>
-      <c r="F31" s="1">
+      <c r="E31" s="1">
         <f t="shared" si="4"/>
         <v>43413</v>
       </c>
-      <c r="G31">
+      <c r="F31">
         <v>0.84415584415584399</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:6">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2814,24 +2618,21 @@
       <c r="B32" t="s">
         <v>24</v>
       </c>
-      <c r="C32">
-        <v>2018</v>
-      </c>
-      <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="3">
         <v>59</v>
       </c>
-      <c r="F32" s="1">
+      <c r="E32" s="1">
         <f t="shared" si="4"/>
         <v>43420</v>
       </c>
-      <c r="G32">
+      <c r="F32">
         <v>0.84415584415584399</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:7">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2839,24 +2640,21 @@
       <c r="B33" t="s">
         <v>24</v>
       </c>
-      <c r="C33">
-        <v>2018</v>
-      </c>
-      <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="3">
         <v>65</v>
       </c>
-      <c r="F33" s="1">
+      <c r="E33" s="1">
         <f t="shared" si="4"/>
         <v>43426</v>
       </c>
-      <c r="G33">
+      <c r="F33">
         <v>0.68181818181818199</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:7">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2864,24 +2662,21 @@
       <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C34">
-        <v>2018</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C34" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="3">
+      <c r="D34" s="3">
         <v>8</v>
       </c>
-      <c r="F34" s="1">
-        <f>$F$24+E34</f>
+      <c r="E34" s="1">
+        <f>$E$24+D34</f>
         <v>43369</v>
       </c>
-      <c r="G34">
+      <c r="F34">
         <v>0.73376623376623396</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:7">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2889,24 +2684,21 @@
       <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="C35">
-        <v>2018</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="3">
+      <c r="D35" s="3">
         <v>16</v>
       </c>
-      <c r="F35" s="1">
-        <f t="shared" ref="F35:F42" si="5">$F$24+E35</f>
+      <c r="E35" s="1">
+        <f t="shared" ref="E35:E42" si="5">$E$24+D35</f>
         <v>43377</v>
       </c>
-      <c r="G35">
+      <c r="F35">
         <v>8.4415584415585096E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:7">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2914,24 +2706,21 @@
       <c r="B36" t="s">
         <v>24</v>
       </c>
-      <c r="C36">
-        <v>2018</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="3">
+      <c r="D36" s="3">
         <v>19</v>
       </c>
-      <c r="F36" s="1">
+      <c r="E36" s="1">
         <f t="shared" si="5"/>
         <v>43380</v>
       </c>
-      <c r="G36">
+      <c r="F36">
         <v>0.103896103896104</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:7">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2939,24 +2728,21 @@
       <c r="B37" t="s">
         <v>24</v>
       </c>
-      <c r="C37">
-        <v>2018</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="3">
-        <v>24</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="D37" s="3">
+        <v>24</v>
+      </c>
+      <c r="E37" s="1">
         <f t="shared" si="5"/>
         <v>43385</v>
       </c>
-      <c r="G37">
+      <c r="F37">
         <v>0.31818181818181801</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:7">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2964,24 +2750,21 @@
       <c r="B38" t="s">
         <v>24</v>
       </c>
-      <c r="C38">
-        <v>2018</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="3">
+      <c r="D38" s="3">
         <v>30</v>
       </c>
-      <c r="F38" s="1">
+      <c r="E38" s="1">
         <f t="shared" si="5"/>
         <v>43391</v>
       </c>
-      <c r="G38">
+      <c r="F38">
         <v>0.415584415584416</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:7">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2989,24 +2772,21 @@
       <c r="B39" t="s">
         <v>24</v>
       </c>
-      <c r="C39">
-        <v>2018</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="3">
+      <c r="D39" s="3">
         <v>43</v>
       </c>
-      <c r="F39" s="1">
+      <c r="E39" s="1">
         <f t="shared" si="5"/>
         <v>43404</v>
       </c>
-      <c r="G39">
+      <c r="F39">
         <v>0.53896103896103897</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:7">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3014,24 +2794,21 @@
       <c r="B40" t="s">
         <v>24</v>
       </c>
-      <c r="C40">
-        <v>2018</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="3">
+      <c r="D40" s="3">
         <v>52</v>
       </c>
-      <c r="F40" s="1">
+      <c r="E40" s="1">
         <f t="shared" si="5"/>
         <v>43413</v>
       </c>
-      <c r="G40">
+      <c r="F40">
         <v>0.61038961038961004</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:7">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3039,24 +2816,21 @@
       <c r="B41" t="s">
         <v>24</v>
       </c>
-      <c r="C41">
-        <v>2018</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="3">
+      <c r="D41" s="3">
         <v>59</v>
       </c>
-      <c r="F41" s="1">
+      <c r="E41" s="1">
         <f t="shared" si="5"/>
         <v>43420</v>
       </c>
-      <c r="G41">
+      <c r="F41">
         <v>0.48051948051948101</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:7">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3064,24 +2838,21 @@
       <c r="B42" t="s">
         <v>24</v>
       </c>
-      <c r="C42">
-        <v>2018</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C42" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="3">
+      <c r="D42" s="3">
         <v>65</v>
       </c>
-      <c r="F42" s="1">
+      <c r="E42" s="1">
         <f t="shared" si="5"/>
         <v>43426</v>
       </c>
-      <c r="G42">
+      <c r="F42">
         <v>0.52597402597402598</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:7">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3089,24 +2860,21 @@
       <c r="B43" t="s">
         <v>24</v>
       </c>
-      <c r="C43">
-        <v>2018</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="3">
+      <c r="D43" s="3">
         <v>30</v>
       </c>
-      <c r="F43" s="1">
-        <f>$F$24+E43</f>
+      <c r="E43" s="1">
+        <f>$E$24+D43</f>
         <v>43391</v>
       </c>
-      <c r="G43">
+      <c r="F43">
         <v>0.75324675324675305</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:7">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3114,24 +2882,21 @@
       <c r="B44" t="s">
         <v>24</v>
       </c>
-      <c r="C44">
-        <v>2018</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C44" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="3">
+      <c r="D44" s="3">
         <v>43</v>
       </c>
-      <c r="F44" s="1">
-        <f t="shared" ref="F44:F47" si="6">$F$24+E44</f>
+      <c r="E44" s="1">
+        <f t="shared" ref="E44:E47" si="6">$E$24+D44</f>
         <v>43404</v>
       </c>
-      <c r="G44">
+      <c r="F44">
         <v>0.29220779220779203</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:7">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3139,24 +2904,21 @@
       <c r="B45" t="s">
         <v>24</v>
       </c>
-      <c r="C45">
-        <v>2018</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="3">
+      <c r="D45" s="3">
         <v>52</v>
       </c>
-      <c r="F45" s="1">
+      <c r="E45" s="1">
         <f t="shared" si="6"/>
         <v>43413</v>
       </c>
-      <c r="G45">
+      <c r="F45">
         <v>0.28571428571428598</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:7">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3164,24 +2926,21 @@
       <c r="B46" t="s">
         <v>24</v>
       </c>
-      <c r="C46">
-        <v>2018</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C46" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="3">
+      <c r="D46" s="3">
         <v>59</v>
       </c>
-      <c r="F46" s="1">
+      <c r="E46" s="1">
         <f t="shared" si="6"/>
         <v>43420</v>
       </c>
-      <c r="G46">
+      <c r="F46">
         <v>0.31168831168831101</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:7">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3189,24 +2948,21 @@
       <c r="B47" t="s">
         <v>24</v>
       </c>
-      <c r="C47">
-        <v>2018</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C47" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="3">
+      <c r="D47" s="3">
         <v>65</v>
       </c>
-      <c r="F47" s="1">
+      <c r="E47" s="1">
         <f t="shared" si="6"/>
         <v>43426</v>
       </c>
-      <c r="G47">
+      <c r="F47">
         <v>0.25974025974025999</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:7">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3214,27 +2970,20 @@
       <c r="B48" t="s">
         <v>24</v>
       </c>
-      <c r="C48">
-        <v>2017</v>
-      </c>
-      <c r="D48" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" s="3">
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="3">
         <v>0</v>
       </c>
-      <c r="F48" s="4">
+      <c r="E48" s="4">
         <v>42985</v>
       </c>
-      <c r="H48">
+      <c r="G48">
         <v>44.198895027624502</v>
       </c>
-      <c r="I48">
-        <f>H48*10</f>
-        <v>441.98895027624502</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3242,28 +2991,21 @@
       <c r="B49" t="s">
         <v>24</v>
       </c>
-      <c r="C49">
-        <v>2017</v>
-      </c>
-      <c r="D49" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="3">
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="3">
         <v>14</v>
       </c>
-      <c r="F49" s="1">
-        <f>$F$48+E49</f>
+      <c r="E49" s="1">
+        <f>$E$48+D49</f>
         <v>42999</v>
       </c>
-      <c r="H49">
+      <c r="G49">
         <v>176.79558011049801</v>
       </c>
-      <c r="I49">
-        <f t="shared" ref="I49:I67" si="7">H49*10</f>
-        <v>1767.9558011049801</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3271,513 +3013,391 @@
       <c r="B50" t="s">
         <v>24</v>
       </c>
-      <c r="C50">
-        <v>2017</v>
-      </c>
-      <c r="D50" t="s">
-        <v>21</v>
-      </c>
-      <c r="E50" s="3">
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="3">
         <v>29</v>
       </c>
-      <c r="F50" s="1">
-        <f t="shared" ref="F50:F57" si="8">$F$48+E50</f>
+      <c r="E50" s="1">
+        <f t="shared" ref="E50:E57" si="7">$E$48+D50</f>
         <v>43014</v>
       </c>
-      <c r="H50">
+      <c r="G50">
         <v>574.58563535911696</v>
       </c>
-      <c r="I50">
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="3">
+        <v>43</v>
+      </c>
+      <c r="E51" s="1">
         <f t="shared" si="7"/>
-        <v>5745.8563535911699</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B51" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51">
-        <v>2017</v>
-      </c>
-      <c r="D51" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="3">
+        <v>43028</v>
+      </c>
+      <c r="G51">
+        <v>1060.7734806629801</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="3">
+        <v>87</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="7"/>
+        <v>43072</v>
+      </c>
+      <c r="G52">
+        <v>2651.93370165745</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Early_WL</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="3">
+        <v>14</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="7"/>
+        <v>42999</v>
+      </c>
+      <c r="G53">
+        <v>88.397790055250795</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Early_WL</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="3">
         <v>43</v>
       </c>
-      <c r="F51" s="1">
+      <c r="E54" s="1">
+        <f t="shared" si="7"/>
+        <v>43028</v>
+      </c>
+      <c r="G54">
+        <v>574.58563535911696</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Early_WL</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="3">
+        <v>87</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="7"/>
+        <v>43072</v>
+      </c>
+      <c r="G55">
+        <v>2232.0441988950201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Late_WL</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="3">
+        <v>43</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="7"/>
+        <v>43028</v>
+      </c>
+      <c r="G56">
+        <v>928.17679558011105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Late_WL</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="3">
+        <v>87</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="7"/>
+        <v>43072</v>
+      </c>
+      <c r="G57">
+        <v>1745.8563535911601</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4">
+        <v>43361</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="3">
+        <v>14</v>
+      </c>
+      <c r="E59" s="1">
+        <f>$E$58+D59</f>
+        <v>43375</v>
+      </c>
+      <c r="G59">
+        <v>309.39226519337302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="3">
+        <v>22</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" ref="E60:E67" si="8">$E$58+D60</f>
+        <v>43383</v>
+      </c>
+      <c r="G60">
+        <v>353.59116022099602</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="3">
+        <v>36</v>
+      </c>
+      <c r="E61" s="1">
         <f t="shared" si="8"/>
-        <v>43028</v>
-      </c>
-      <c r="H51">
-        <v>1060.7734806629801</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="7"/>
-        <v>10607.7348066298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52">
-        <v>2017</v>
-      </c>
-      <c r="D52" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="3">
-        <v>87</v>
-      </c>
-      <c r="F52" s="1">
+        <v>43397</v>
+      </c>
+      <c r="G61">
+        <v>795.58011049723905</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="str">
+        <f t="shared" si="0"/>
+        <v>Exp_1_Control</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="3">
+        <v>79</v>
+      </c>
+      <c r="E62" s="1">
         <f t="shared" si="8"/>
-        <v>43072</v>
-      </c>
-      <c r="H52">
-        <v>2651.93370165745</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="7"/>
-        <v>26519.3370165745</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="str">
+        <v>43440</v>
+      </c>
+      <c r="G62">
+        <v>2033.14917127071</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
       </c>
-      <c r="B53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53">
-        <v>2017</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="3">
+      <c r="D63" s="3">
         <v>14</v>
       </c>
-      <c r="F53" s="1">
+      <c r="E63" s="1">
         <f t="shared" si="8"/>
-        <v>42999</v>
-      </c>
-      <c r="H53">
-        <v>88.397790055250795</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="7"/>
-        <v>883.97790055250789</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="str">
+        <v>43375</v>
+      </c>
+      <c r="G63">
+        <v>132.59668508287501</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
       </c>
-      <c r="B54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54">
-        <v>2017</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="3">
-        <v>43</v>
-      </c>
-      <c r="F54" s="1">
+      <c r="D64" s="3">
+        <v>36</v>
+      </c>
+      <c r="E64" s="1">
         <f t="shared" si="8"/>
-        <v>43028</v>
-      </c>
-      <c r="H54">
-        <v>574.58563535911696</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="7"/>
-        <v>5745.8563535911699</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="str">
+        <v>43397</v>
+      </c>
+      <c r="G64">
+        <v>176.79558011049801</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
       </c>
-      <c r="B55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55">
-        <v>2017</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="3">
-        <v>87</v>
-      </c>
-      <c r="F55" s="1">
+      <c r="D65" s="3">
+        <v>79</v>
+      </c>
+      <c r="E65" s="1">
         <f t="shared" si="8"/>
-        <v>43072</v>
-      </c>
-      <c r="H55">
-        <v>2232.0441988950201</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="7"/>
-        <v>22320.441988950202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" t="str">
+        <v>43440</v>
+      </c>
+      <c r="G65">
+        <v>1480.6629834254099</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
       </c>
-      <c r="B56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56">
-        <v>2017</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" t="s">
         <v>27</v>
       </c>
-      <c r="E56" s="3">
-        <v>43</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="D66" s="3">
+        <v>36</v>
+      </c>
+      <c r="E66" s="1">
         <f t="shared" si="8"/>
-        <v>43028</v>
-      </c>
-      <c r="H56">
-        <v>928.17679558011105</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="7"/>
-        <v>9281.7679558011114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="str">
-        <f t="shared" si="0"/>
+        <v>43397</v>
+      </c>
+      <c r="G66">
+        <v>596.685082872929</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="str">
+        <f t="shared" ref="A67" si="9">"Exp_1_"&amp;C67</f>
         <v>Exp_1_Late_WL</v>
       </c>
-      <c r="B57" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57">
-        <v>2017</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
         <v>27</v>
       </c>
-      <c r="E57" s="3">
-        <v>87</v>
-      </c>
-      <c r="F57" s="1">
+      <c r="D67" s="3">
+        <v>79</v>
+      </c>
+      <c r="E67" s="1">
         <f t="shared" si="8"/>
-        <v>43072</v>
-      </c>
-      <c r="H57">
-        <v>1745.8563535911601</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="7"/>
-        <v>17458.563535911602</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58">
-        <v>2018</v>
-      </c>
-      <c r="D58" t="s">
-        <v>21</v>
-      </c>
-      <c r="E58" s="3">
-        <v>0</v>
-      </c>
-      <c r="F58" s="4">
-        <v>43361</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59">
-        <v>2018</v>
-      </c>
-      <c r="D59" t="s">
-        <v>21</v>
-      </c>
-      <c r="E59" s="3">
-        <v>14</v>
-      </c>
-      <c r="F59" s="1">
-        <f>$F$58+E59</f>
-        <v>43375</v>
-      </c>
-      <c r="H59">
-        <v>309.39226519337302</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="7"/>
-        <v>3093.9226519337303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B60" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60">
-        <v>2018</v>
-      </c>
-      <c r="D60" t="s">
-        <v>21</v>
-      </c>
-      <c r="E60" s="3">
-        <v>22</v>
-      </c>
-      <c r="F60" s="1">
-        <f t="shared" ref="F60:F67" si="9">$F$58+E60</f>
-        <v>43383</v>
-      </c>
-      <c r="H60">
-        <v>353.59116022099602</v>
-      </c>
-      <c r="I60">
-        <f t="shared" si="7"/>
-        <v>3535.9116022099602</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B61" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61">
-        <v>2018</v>
-      </c>
-      <c r="D61" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="3">
-        <v>36</v>
-      </c>
-      <c r="F61" s="1">
-        <f t="shared" si="9"/>
-        <v>43397</v>
-      </c>
-      <c r="H61">
+        <v>43440</v>
+      </c>
+      <c r="G67">
         <v>795.58011049723905</v>
-      </c>
-      <c r="I61">
-        <f t="shared" si="7"/>
-        <v>7955.80110497239</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Control</v>
-      </c>
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62">
-        <v>2018</v>
-      </c>
-      <c r="D62" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="3">
-        <v>79</v>
-      </c>
-      <c r="F62" s="1">
-        <f t="shared" si="9"/>
-        <v>43440</v>
-      </c>
-      <c r="H62">
-        <v>2033.14917127071</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="7"/>
-        <v>20331.491712707098</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Early_WL</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63">
-        <v>2018</v>
-      </c>
-      <c r="D63" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" s="3">
-        <v>14</v>
-      </c>
-      <c r="F63" s="1">
-        <f t="shared" si="9"/>
-        <v>43375</v>
-      </c>
-      <c r="H63">
-        <v>132.59668508287501</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="7"/>
-        <v>1325.96685082875</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Early_WL</v>
-      </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64">
-        <v>2018</v>
-      </c>
-      <c r="D64" t="s">
-        <v>26</v>
-      </c>
-      <c r="E64" s="3">
-        <v>36</v>
-      </c>
-      <c r="F64" s="1">
-        <f t="shared" si="9"/>
-        <v>43397</v>
-      </c>
-      <c r="H64">
-        <v>176.79558011049801</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="7"/>
-        <v>1767.9558011049801</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Early_WL</v>
-      </c>
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65">
-        <v>2018</v>
-      </c>
-      <c r="D65" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" s="3">
-        <v>79</v>
-      </c>
-      <c r="F65" s="1">
-        <f t="shared" si="9"/>
-        <v>43440</v>
-      </c>
-      <c r="H65">
-        <v>1480.6629834254099</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="7"/>
-        <v>14806.629834254099</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" t="str">
-        <f t="shared" si="0"/>
-        <v>Exp_1_Late_WL</v>
-      </c>
-      <c r="B66" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66">
-        <v>2018</v>
-      </c>
-      <c r="D66" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="3">
-        <v>36</v>
-      </c>
-      <c r="F66" s="1">
-        <f t="shared" si="9"/>
-        <v>43397</v>
-      </c>
-      <c r="H66">
-        <v>596.685082872929</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="7"/>
-        <v>5966.8508287292898</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" t="str">
-        <f t="shared" ref="A67" si="10">"Exp_1_"&amp;D67</f>
-        <v>Exp_1_Late_WL</v>
-      </c>
-      <c r="B67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67">
-        <v>2018</v>
-      </c>
-      <c r="D67" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="3">
-        <v>79</v>
-      </c>
-      <c r="F67" s="1">
-        <f t="shared" si="9"/>
-        <v>43440</v>
-      </c>
-      <c r="H67">
-        <v>795.58011049723905</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="7"/>
-        <v>7955.80110497239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove variables we weren't supposed to include.
The CoverGreen variable was a proxy for a different value APSIM does not
predict during calibration.
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/ObsPloschuk2021.xlsx
+++ b/Tests/Validation/Canola/ObsPloschuk2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilhuber\NextGen\ApsimX\Tests\Validation\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B7C8FA-AE9A-43F2-95BC-323A83DDBB69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1133681F-7E4E-4BE1-88BF-0DD3CFD90A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="2430" windowWidth="28800" windowHeight="13050" activeTab="4" xr2:uid="{03D29272-A8D3-49D2-9408-6969D9C41BBD}"/>
+    <workbookView xWindow="10080" yWindow="2430" windowWidth="28800" windowHeight="13050" activeTab="1" xr2:uid="{03D29272-A8D3-49D2-9408-6969D9C41BBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Canola" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">LAI_at_end_treatment!$A$1:$F$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RUE_at_end_treatment!$A$1:$E$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TimeSeries!$A$1:$G$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TimeSeries!$A$1:$F$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="36">
   <si>
     <t>LAI</t>
   </si>
@@ -135,13 +135,7 @@
     <t>Canola.Aboveground.Wt</t>
   </si>
   <si>
-    <t>Canola.Grain.HarvestIndex</t>
-  </si>
-  <si>
     <t>Canola.Grain.HarvestIndexError</t>
-  </si>
-  <si>
-    <t>Canola.Leaf.CoverGreen</t>
   </si>
   <si>
     <t>Canola.Grain.Wt</t>
@@ -540,7 +534,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -879,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCE79FF-CA68-45F5-80EF-0981CBC1EC45}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -895,19 +889,18 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -921,10 +914,10 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -936,28 +929,25 @@
         <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" t="str">
         <f>"Exp_1_"&amp;D2</f>
         <v>Exp_1_Control</v>
@@ -984,31 +974,28 @@
         <v>7967.4337148168352</v>
       </c>
       <c r="I2">
-        <v>0.27700000000000002</v>
+        <v>1.0392304845413263E-2</v>
       </c>
       <c r="J2">
-        <v>1.0392304845413263E-2</v>
+        <v>11239</v>
       </c>
       <c r="K2">
-        <v>11239</v>
+        <v>277.12812921102034</v>
       </c>
       <c r="L2">
-        <v>277.12812921102034</v>
+        <v>15.7</v>
       </c>
       <c r="M2">
-        <v>15.7</v>
+        <v>1.0392304845413263</v>
       </c>
       <c r="N2">
-        <v>1.0392304845413263</v>
+        <v>3.7</v>
       </c>
       <c r="O2">
-        <v>3.7</v>
-      </c>
-      <c r="P2">
         <v>0.17320508075688773</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A7" si="0">"Exp_1_"&amp;D3</f>
         <v>Exp_1_Early_WL</v>
@@ -1035,31 +1022,28 @@
         <v>15761.662348876782</v>
       </c>
       <c r="I3">
-        <v>0.23899999999999999</v>
+        <v>1.9052558883257648E-2</v>
       </c>
       <c r="J3">
-        <v>1.9052558883257648E-2</v>
+        <v>9945</v>
       </c>
       <c r="K3">
-        <v>9945</v>
+        <v>162.81277591147446</v>
       </c>
       <c r="L3">
-        <v>162.81277591147446</v>
+        <v>14.3</v>
       </c>
       <c r="M3">
-        <v>14.3</v>
+        <v>2.9444863728670914</v>
       </c>
       <c r="N3">
-        <v>2.9444863728670914</v>
+        <v>3.7</v>
       </c>
       <c r="O3">
-        <v>3.7</v>
-      </c>
-      <c r="P3">
         <v>0.34641016151377546</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1086,31 +1070,28 @@
         <v>5369.3575034635196</v>
       </c>
       <c r="I4">
-        <v>0.223</v>
+        <v>1.212435565298214E-2</v>
       </c>
       <c r="J4">
-        <v>1.212435565298214E-2</v>
+        <v>10828</v>
       </c>
       <c r="K4">
-        <v>10828</v>
+        <v>495.36653096469888</v>
       </c>
       <c r="L4">
-        <v>495.36653096469888</v>
+        <v>10.1</v>
       </c>
       <c r="M4">
-        <v>10.1</v>
+        <v>0.51961524227066314</v>
       </c>
       <c r="N4">
-        <v>0.51961524227066314</v>
+        <v>3.4</v>
       </c>
       <c r="O4">
-        <v>3.4</v>
-      </c>
-      <c r="P4">
         <v>0.17320508075688773</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:15">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -1137,31 +1118,28 @@
         <v>28059.223082615812</v>
       </c>
       <c r="I5">
-        <v>0.30499999999999999</v>
+        <v>1.0392304845413263E-2</v>
       </c>
       <c r="J5">
-        <v>1.0392304845413263E-2</v>
+        <v>13150</v>
       </c>
       <c r="K5">
-        <v>13150</v>
+        <v>3363.6426682987594</v>
       </c>
       <c r="L5">
-        <v>3363.6426682987594</v>
+        <v>13.3</v>
       </c>
       <c r="M5">
-        <v>13.3</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="N5">
-        <v>0.8660254037844386</v>
+        <v>3.7</v>
       </c>
       <c r="O5">
-        <v>3.7</v>
-      </c>
-      <c r="P5">
         <v>0.17320508075688773</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:15">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -1188,31 +1166,28 @@
         <v>19398.969044771424</v>
       </c>
       <c r="I6">
-        <v>0.30499999999999999</v>
+        <v>8.6602540378443865E-3</v>
       </c>
       <c r="J6">
-        <v>8.6602540378443865E-3</v>
+        <v>10457</v>
       </c>
       <c r="K6">
-        <v>10457</v>
+        <v>2346.9288442558286</v>
       </c>
       <c r="L6">
-        <v>2346.9288442558286</v>
+        <v>12.7</v>
       </c>
       <c r="M6">
-        <v>12.7</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="N6">
-        <v>0.8660254037844386</v>
+        <v>3.4</v>
       </c>
       <c r="O6">
-        <v>3.4</v>
-      </c>
-      <c r="P6">
         <v>0.17320508075688773</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:15">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -1239,27 +1214,24 @@
         <v>14202.816622064793</v>
       </c>
       <c r="I7">
-        <v>0.23899999999999999</v>
+        <v>2.5980762113533156E-2</v>
       </c>
       <c r="J7">
-        <v>2.5980762113533156E-2</v>
+        <v>6353</v>
       </c>
       <c r="K7">
-        <v>6353</v>
+        <v>1988.3943270890711</v>
       </c>
       <c r="L7">
-        <v>1988.3943270890711</v>
+        <v>9.4</v>
       </c>
       <c r="M7">
-        <v>9.4</v>
+        <v>0.69282032302755092</v>
       </c>
       <c r="N7">
-        <v>0.69282032302755092</v>
+        <v>3.2</v>
       </c>
       <c r="O7">
-        <v>3.2</v>
-      </c>
-      <c r="P7">
         <v>0.34641016151377546</v>
       </c>
     </row>
@@ -1273,7 +1245,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1523,13 +1495,14 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1917,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCDE50D-DC28-4398-95CA-92F7BC129FD5}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1929,7 +1902,7 @@
     <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1946,13 +1919,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" t="str">
         <f>"Exp_1_"&amp;C2</f>
         <v>Exp_1_Control</v>
@@ -1969,11 +1939,8 @@
       <c r="E2" s="4">
         <v>42985</v>
       </c>
-      <c r="F2">
-        <v>0.57788944723618096</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">"Exp_1_"&amp;C3</f>
         <v>Exp_1_Control</v>
@@ -1991,11 +1958,8 @@
         <f>$E$2+D3</f>
         <v>42994</v>
       </c>
-      <c r="F3">
-        <v>0.91959798994974795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2013,11 +1977,8 @@
         <f t="shared" ref="E4:E9" si="1">$E$2+D4</f>
         <v>43018</v>
       </c>
-      <c r="F4">
-        <v>0.95477386934673303</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2035,11 +1996,8 @@
         <f t="shared" si="1"/>
         <v>43031</v>
       </c>
-      <c r="F5">
-        <v>0.96482412060301503</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2057,11 +2015,8 @@
         <f t="shared" si="1"/>
         <v>43034</v>
       </c>
-      <c r="F6">
-        <v>0.904522613065326</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2079,11 +2034,8 @@
         <f t="shared" si="1"/>
         <v>43042</v>
       </c>
-      <c r="F7">
-        <v>0.89447236180904399</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2101,11 +2053,8 @@
         <f t="shared" si="1"/>
         <v>43051</v>
       </c>
-      <c r="F8">
-        <v>0.82412060301507495</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2123,11 +2072,8 @@
         <f t="shared" si="1"/>
         <v>43056</v>
       </c>
-      <c r="F9">
-        <v>0.67839195979899403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2145,11 +2091,8 @@
         <f>$E$2+D10</f>
         <v>42995</v>
       </c>
-      <c r="F10">
-        <v>0.56281407035175901</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2167,11 +2110,8 @@
         <f t="shared" ref="E11:E17" si="2">$E$2+D11</f>
         <v>43001</v>
       </c>
-      <c r="F11">
-        <v>0.41708542713567798</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2189,11 +2129,8 @@
         <f t="shared" si="2"/>
         <v>43018</v>
       </c>
-      <c r="F12">
-        <v>0.86934673366834103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2211,11 +2148,8 @@
         <f t="shared" si="2"/>
         <v>43031</v>
       </c>
-      <c r="F13">
-        <v>0.80904522613065299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2233,11 +2167,8 @@
         <f t="shared" si="2"/>
         <v>43035</v>
       </c>
-      <c r="F14">
-        <v>0.85929648241206003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2255,11 +2186,8 @@
         <f t="shared" si="2"/>
         <v>43042</v>
       </c>
-      <c r="F15">
-        <v>0.81407035175879405</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2277,11 +2205,8 @@
         <f t="shared" si="2"/>
         <v>43051</v>
       </c>
-      <c r="F16">
-        <v>0.85929648241206003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2299,11 +2224,8 @@
         <f t="shared" si="2"/>
         <v>43057</v>
       </c>
-      <c r="F17">
-        <v>0.80904522613065299</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2321,11 +2243,8 @@
         <f>$E$2+D18</f>
         <v>43017</v>
       </c>
-      <c r="F18">
-        <v>0.904522613065326</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2343,11 +2262,8 @@
         <f t="shared" ref="E19:E23" si="3">$E$2+D19</f>
         <v>43031</v>
       </c>
-      <c r="F19">
-        <v>0.51758793969849204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2365,11 +2281,8 @@
         <f t="shared" si="3"/>
         <v>43035</v>
       </c>
-      <c r="F20">
-        <v>0.32663316582914498</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2387,11 +2300,8 @@
         <f t="shared" si="3"/>
         <v>43042</v>
       </c>
-      <c r="F21">
-        <v>0.33668341708542598</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2409,11 +2319,8 @@
         <f t="shared" si="3"/>
         <v>43052</v>
       </c>
-      <c r="F22">
-        <v>0.46733668341708501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2431,11 +2338,8 @@
         <f t="shared" si="3"/>
         <v>43057</v>
       </c>
-      <c r="F23">
-        <v>0.34170854271356699</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2452,11 +2356,8 @@
       <c r="E24" s="4">
         <v>43361</v>
       </c>
-      <c r="F24">
-        <v>0.25974025974025999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2474,11 +2375,8 @@
         <f>$E$24+D25</f>
         <v>43369</v>
       </c>
-      <c r="F25">
-        <v>0.74025974025973995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2496,11 +2394,8 @@
         <f t="shared" ref="E26:E33" si="4">$E$24+D26</f>
         <v>43377</v>
       </c>
-      <c r="F26">
-        <v>0.92207792207792205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2518,11 +2413,8 @@
         <f t="shared" si="4"/>
         <v>43380</v>
       </c>
-      <c r="F27">
-        <v>0.89610389610389596</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2540,11 +2432,8 @@
         <f t="shared" si="4"/>
         <v>43385</v>
       </c>
-      <c r="F28">
-        <v>0.92857142857142905</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2562,11 +2451,8 @@
         <f t="shared" si="4"/>
         <v>43391</v>
       </c>
-      <c r="F29">
-        <v>0.95454545454545503</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2584,11 +2470,8 @@
         <f t="shared" si="4"/>
         <v>43404</v>
       </c>
-      <c r="F30">
-        <v>0.84415584415584399</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2606,11 +2489,8 @@
         <f t="shared" si="4"/>
         <v>43413</v>
       </c>
-      <c r="F31">
-        <v>0.84415584415584399</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2628,11 +2508,8 @@
         <f t="shared" si="4"/>
         <v>43420</v>
       </c>
-      <c r="F32">
-        <v>0.84415584415584399</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2650,11 +2527,8 @@
         <f t="shared" si="4"/>
         <v>43426</v>
       </c>
-      <c r="F33">
-        <v>0.68181818181818199</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2672,11 +2546,8 @@
         <f>$E$24+D34</f>
         <v>43369</v>
       </c>
-      <c r="F34">
-        <v>0.73376623376623396</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2694,11 +2565,8 @@
         <f t="shared" ref="E35:E42" si="5">$E$24+D35</f>
         <v>43377</v>
       </c>
-      <c r="F35">
-        <v>8.4415584415585096E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2716,11 +2584,8 @@
         <f t="shared" si="5"/>
         <v>43380</v>
       </c>
-      <c r="F36">
-        <v>0.103896103896104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2738,11 +2603,8 @@
         <f t="shared" si="5"/>
         <v>43385</v>
       </c>
-      <c r="F37">
-        <v>0.31818181818181801</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2760,11 +2622,8 @@
         <f t="shared" si="5"/>
         <v>43391</v>
       </c>
-      <c r="F38">
-        <v>0.415584415584416</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2782,11 +2641,8 @@
         <f t="shared" si="5"/>
         <v>43404</v>
       </c>
-      <c r="F39">
-        <v>0.53896103896103897</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2804,11 +2660,8 @@
         <f t="shared" si="5"/>
         <v>43413</v>
       </c>
-      <c r="F40">
-        <v>0.61038961038961004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2826,11 +2679,8 @@
         <f t="shared" si="5"/>
         <v>43420</v>
       </c>
-      <c r="F41">
-        <v>0.48051948051948101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -2848,11 +2698,8 @@
         <f t="shared" si="5"/>
         <v>43426</v>
       </c>
-      <c r="F42">
-        <v>0.52597402597402598</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2870,11 +2717,8 @@
         <f>$E$24+D43</f>
         <v>43391</v>
       </c>
-      <c r="F43">
-        <v>0.75324675324675305</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2892,11 +2736,8 @@
         <f t="shared" ref="E44:E47" si="6">$E$24+D44</f>
         <v>43404</v>
       </c>
-      <c r="F44">
-        <v>0.29220779220779203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2914,11 +2755,8 @@
         <f t="shared" si="6"/>
         <v>43413</v>
       </c>
-      <c r="F45">
-        <v>0.28571428571428598</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2936,11 +2774,8 @@
         <f t="shared" si="6"/>
         <v>43420</v>
       </c>
-      <c r="F46">
-        <v>0.31168831168831101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -2958,11 +2793,8 @@
         <f t="shared" si="6"/>
         <v>43426</v>
       </c>
-      <c r="F47">
-        <v>0.25974025974025999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -2979,11 +2811,11 @@
       <c r="E48" s="4">
         <v>42985</v>
       </c>
-      <c r="G48">
+      <c r="F48">
         <v>44.198895027624502</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:6">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3001,11 +2833,11 @@
         <f>$E$48+D49</f>
         <v>42999</v>
       </c>
-      <c r="G49">
+      <c r="F49">
         <v>176.79558011049801</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:6">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3023,11 +2855,11 @@
         <f t="shared" ref="E50:E57" si="7">$E$48+D50</f>
         <v>43014</v>
       </c>
-      <c r="G50">
+      <c r="F50">
         <v>574.58563535911696</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:6">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3045,11 +2877,11 @@
         <f t="shared" si="7"/>
         <v>43028</v>
       </c>
-      <c r="G51">
+      <c r="F51">
         <v>1060.7734806629801</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:6">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3067,11 +2899,11 @@
         <f t="shared" si="7"/>
         <v>43072</v>
       </c>
-      <c r="G52">
+      <c r="F52">
         <v>2651.93370165745</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:6">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3089,11 +2921,11 @@
         <f t="shared" si="7"/>
         <v>42999</v>
       </c>
-      <c r="G53">
+      <c r="F53">
         <v>88.397790055250795</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:6">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3111,11 +2943,11 @@
         <f t="shared" si="7"/>
         <v>43028</v>
       </c>
-      <c r="G54">
+      <c r="F54">
         <v>574.58563535911696</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:6">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3133,11 +2965,11 @@
         <f t="shared" si="7"/>
         <v>43072</v>
       </c>
-      <c r="G55">
+      <c r="F55">
         <v>2232.0441988950201</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:6">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3155,11 +2987,11 @@
         <f t="shared" si="7"/>
         <v>43028</v>
       </c>
-      <c r="G56">
+      <c r="F56">
         <v>928.17679558011105</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:6">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3177,11 +3009,11 @@
         <f t="shared" si="7"/>
         <v>43072</v>
       </c>
-      <c r="G57">
+      <c r="F57">
         <v>1745.8563535911601</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:6">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3198,11 +3030,11 @@
       <c r="E58" s="4">
         <v>43361</v>
       </c>
-      <c r="G58">
+      <c r="F58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:6">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3220,11 +3052,11 @@
         <f>$E$58+D59</f>
         <v>43375</v>
       </c>
-      <c r="G59">
+      <c r="F59">
         <v>309.39226519337302</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:6">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3242,11 +3074,11 @@
         <f t="shared" ref="E60:E67" si="8">$E$58+D60</f>
         <v>43383</v>
       </c>
-      <c r="G60">
+      <c r="F60">
         <v>353.59116022099602</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:6">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3264,11 +3096,11 @@
         <f t="shared" si="8"/>
         <v>43397</v>
       </c>
-      <c r="G61">
+      <c r="F61">
         <v>795.58011049723905</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:6">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Control</v>
@@ -3286,11 +3118,11 @@
         <f t="shared" si="8"/>
         <v>43440</v>
       </c>
-      <c r="G62">
+      <c r="F62">
         <v>2033.14917127071</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:6">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3308,11 +3140,11 @@
         <f t="shared" si="8"/>
         <v>43375</v>
       </c>
-      <c r="G63">
+      <c r="F63">
         <v>132.59668508287501</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:6">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3330,11 +3162,11 @@
         <f t="shared" si="8"/>
         <v>43397</v>
       </c>
-      <c r="G64">
+      <c r="F64">
         <v>176.79558011049801</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:6">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Early_WL</v>
@@ -3352,11 +3184,11 @@
         <f t="shared" si="8"/>
         <v>43440</v>
       </c>
-      <c r="G65">
+      <c r="F65">
         <v>1480.6629834254099</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:6">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Exp_1_Late_WL</v>
@@ -3374,11 +3206,11 @@
         <f t="shared" si="8"/>
         <v>43397</v>
       </c>
-      <c r="G66">
+      <c r="F66">
         <v>596.685082872929</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:6">
       <c r="A67" t="str">
         <f t="shared" ref="A67" si="9">"Exp_1_"&amp;C67</f>
         <v>Exp_1_Late_WL</v>
@@ -3396,7 +3228,7 @@
         <f t="shared" si="8"/>
         <v>43440</v>
       </c>
-      <c r="G67">
+      <c r="F67">
         <v>795.58011049723905</v>
       </c>
     </row>

</xml_diff>